<commit_message>
Added Successful, Failed, and Skipped counter in spreadsheet.
</commit_message>
<xml_diff>
--- a/file_renaming_report.xlsx
+++ b/file_renaming_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jicap-my.sharepoint.com/personal/hamza_ahmed_jicap-performance_com/Documents/auto-renamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_A8C8B5A59859CE0F62355476585DCE3A17C423F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{055BB801-D938-0B4F-9382-DD7244FA26F6}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_A8C8B5A59859CE0F62355476585DCE3A17C423F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DF565D8-385D-D841-BCDD-7D06C4CC5003}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36060" yWindow="1240" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File Processing Report" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'File Processing Report'!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="339">
   <si>
     <t>Original Filename</t>
   </si>
@@ -1031,13 +1044,22 @@
   </si>
   <si>
     <t>Site number changed</t>
+  </si>
+  <si>
+    <t>Count Successful</t>
+  </si>
+  <si>
+    <t>Count Fail</t>
+  </si>
+  <si>
+    <t>Count Skipped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1050,6 +1072,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1093,12 +1123,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1401,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D180"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1446,7 @@
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1436,8 +1467,15 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(C:C, "Successful")</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1447,8 +1485,15 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3">
+        <f>COUNTIF(C:C, "Failed")</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>321</v>
       </c>
@@ -1458,8 +1503,15 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4">
+        <f>COUNTIF(C:C, "Skipped")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -1470,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1481,7 +1533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -1492,7 +1544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -1514,7 +1566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -1525,7 +1577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -1536,7 +1588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -1547,7 +1599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1558,7 +1610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>244</v>
       </c>
@@ -1569,7 +1621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>198</v>
       </c>
@@ -1580,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>114</v>
       </c>

</xml_diff>